<commit_message>
added information from coders
</commit_message>
<xml_diff>
--- a/analysis/second_coder_done.xlsx
+++ b/analysis/second_coder_done.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/erinbuchanan/GitHub/Research/2_projects/Transparency-Ling/analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCE0A161-FC1D-6C43-880E-8F8B4FC0DB4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D670E0FE-5669-304D-97A7-3BF5DE329661}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-20" yWindow="780" windowWidth="30240" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="second_coder_check" sheetId="1" r:id="rId1"/>
@@ -2078,7 +2078,7 @@
   <dimension ref="A1:I3361"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -79290,6 +79290,7 @@
     <sortCondition ref="B2:B3361"/>
   </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 

</xml_diff>